<commit_message>
auto AGV push away
</commit_message>
<xml_diff>
--- a/data/epsp/demo/2x(6+2).xlsx
+++ b/data/epsp/demo/2x(6+2).xlsx
@@ -22,10 +22,10 @@
     <t>Start|1</t>
   </si>
   <si>
-    <t>Tank1|2</t>
-  </si>
-  <si>
-    <t>Tank2|3</t>
+    <t>Tank1|3</t>
+  </si>
+  <si>
+    <t>Tank2|4</t>
   </si>
   <si>
     <t>Tank3|6</t>
@@ -37,7 +37,7 @@
     <t>End|9</t>
   </si>
   <si>
-    <t>AGV1|1</t>
+    <t>AGV1|2</t>
   </si>
   <si>
     <t>AGV2|8</t>
@@ -457,7 +457,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -489,10 +489,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -573,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -605,10 +605,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>

</xml_diff>